<commit_message>
data, gnuplot euler, update each code for exact solution
</commit_message>
<xml_diff>
--- a/Calc-Results.xlsx
+++ b/Calc-Results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUREM\ITS\SEM 5\ANUM\anum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ADD24D-1A7E-449E-89AB-333148F1E3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BF0624-0A1E-4CDC-8DD2-EF7477099DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E12C029A-BF25-4C4F-9CE7-3942E7EFC98C}"/>
+    <workbookView xWindow="765" yWindow="2295" windowWidth="12510" windowHeight="11295" xr2:uid="{E12C029A-BF25-4C4F-9CE7-3942E7EFC98C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IVP2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0000000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -113,10 +113,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -437,7 +437,7 @@
   <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,288 +475,288 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="D3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3">
         <v>0.1</v>
       </c>
-      <c r="G3" s="2">
-        <v>147.46192271000001</v>
+      <c r="G3" s="1">
+        <v>6.4161886868000007E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4">
         <v>0.01</v>
       </c>
-      <c r="G4" s="2">
-        <v>147.46963163000001</v>
+      <c r="G4" s="1">
+        <v>6.3939021303999997E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5">
         <v>1E-3</v>
       </c>
-      <c r="G5" s="2">
-        <v>147.4702643</v>
+      <c r="G5" s="1">
+        <v>6.3863691130000002E-4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6">
         <v>0.1</v>
       </c>
-      <c r="G6" s="2">
-        <v>147.4131591</v>
+      <c r="G6" s="1">
+        <v>0.43526659838999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7">
         <v>0.01</v>
       </c>
-      <c r="G7" s="2">
-        <v>147.41029760000001</v>
+      <c r="G7" s="1">
+        <v>1.9467951075999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8">
         <v>1E-3</v>
       </c>
-      <c r="G8" s="2">
-        <v>147.40983262</v>
+      <c r="G8" s="1">
+        <v>1.8493303035E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>5</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9">
         <v>0.1</v>
       </c>
-      <c r="G9" s="2">
-        <v>147.47667114999999</v>
+      <c r="G9" s="1">
+        <v>9.1636700379999995E-3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10">
         <v>0.01</v>
       </c>
-      <c r="G10" s="2">
-        <v>147.47038941</v>
+      <c r="G10" s="1">
+        <v>1.0831145445E-4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="2">
-        <v>147.47033404000001</v>
+      <c r="G11" s="1">
+        <v>1.1042980272E-6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
         <v>5</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12">
         <v>0.1</v>
       </c>
-      <c r="G12" s="2">
-        <v>147.40779527000001</v>
+      <c r="G12" s="1">
+        <v>6.4733401605999996E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13">
         <v>0.01</v>
       </c>
-      <c r="G13" s="2">
-        <v>147.40976687</v>
+      <c r="G13" s="1">
+        <v>6.4334177176999998E-4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
       <c r="F14">
         <v>1E-3</v>
       </c>
-      <c r="G14" s="2">
-        <v>147.40977863000001</v>
+      <c r="G14" s="1">
+        <v>6.0553736940000002E-6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="D15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="2">
         <v>1</v>
       </c>
       <c r="F15">
         <v>0.1</v>
       </c>
-      <c r="G15" s="2">
-        <v>147.47038380000001</v>
+      <c r="G15" s="1">
+        <v>6.3326523132999996E-5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
       <c r="F16">
         <v>0.01</v>
       </c>
-      <c r="G16" s="2">
-        <v>147.47033349</v>
+      <c r="G16" s="1">
+        <v>7.6208883648000007E-9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17">
         <v>1E-3</v>
       </c>
-      <c r="G17" s="2">
-        <v>147.47033347999999</v>
+      <c r="G17" s="1">
+        <v>7.7637896111999998E-13</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>2</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18">
         <v>0.1</v>
       </c>
-      <c r="G18" s="2">
-        <v>147.40976011000001</v>
+      <c r="G18" s="1">
+        <v>3.4273915798999999E-4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
       <c r="F19">
         <v>0.01</v>
       </c>
-      <c r="G19" s="2">
-        <v>147.40977874000001</v>
+      <c r="G19" s="1">
+        <v>2.6969156730000001E-7</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
       <c r="F20">
         <v>1E-3</v>
       </c>
-      <c r="G20" s="2">
-        <v>147.40977874000001</v>
+      <c r="G20" s="1">
+        <v>2.6141755427000001E-11</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -766,23 +766,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
@@ -793,6 +776,23 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="B3:B5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>